<commit_message>
updated cost and time sheet
</commit_message>
<xml_diff>
--- a/Documentation/ShoaibStatistics/cost-and-time.xlsx
+++ b/Documentation/ShoaibStatistics/cost-and-time.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="19020" windowHeight="8325" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="19020" windowHeight="8325" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="cost" sheetId="1" r:id="rId1"/>
+    <sheet name="time" sheetId="2" r:id="rId2"/>
+    <sheet name="cost breakdown" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>Automation</t>
   </si>
@@ -88,16 +88,103 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Instance hours</t>
+  </si>
+  <si>
+    <t>Total Charged Cost:</t>
+  </si>
+  <si>
+    <t>Experiments</t>
+  </si>
+  <si>
+    <t>Total Slave Hours</t>
+  </si>
+  <si>
+    <t>Total Master Hours:</t>
+  </si>
+  <si>
+    <t>total seconds</t>
+  </si>
+  <si>
+    <t>total hours</t>
+  </si>
+  <si>
+    <t>Total EC2 Slave Cost: 
+@ $0.11 / hour</t>
+  </si>
+  <si>
+    <t>Total EC2 Master Cost:
+@ $0.11 / hour</t>
+  </si>
+  <si>
+    <t>Total S3 data transfer cost:
+@ $0.005 /thousand transfer</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Total </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Variable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Cost (EC2+S3):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Total </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fixed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Cost (EBS + AMI):
+@ $0.01 GB-Month</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +197,21 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -144,7 +246,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -230,11 +332,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -273,8 +456,77 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -291,20 +543,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>67831</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -323,8 +575,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6048375" y="952500"/>
-          <a:ext cx="4791075" cy="3905250"/>
+          <a:off x="609600" y="7239000"/>
+          <a:ext cx="10058400" cy="5020831"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -333,33 +585,28 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>67831</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="4" name="Picture 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -372,8 +619,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609600" y="2552700"/>
-          <a:ext cx="10058400" cy="5020831"/>
+          <a:off x="609600" y="190500"/>
+          <a:ext cx="9772650" cy="6429375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -672,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D12"/>
+  <dimension ref="B3:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,9 +930,17 @@
     <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -693,24 +948,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="9">
-        <v>1.93</v>
+        <v>2.35</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="7"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>0</v>
       </c>
@@ -718,7 +973,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
@@ -726,7 +981,7 @@
         <v>2115</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
@@ -734,7 +989,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
@@ -742,7 +997,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
@@ -750,7 +1005,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>2</v>
       </c>
@@ -758,18 +1013,213 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="8">
         <v>988</v>
       </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13">
+        <f>SUM(C6:C12)</f>
+        <v>5532</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <f>C13/60/60</f>
+        <v>1.5366666666666666</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="23"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F16" s="18"/>
+      <c r="G16" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="18"/>
+    </row>
+    <row r="17" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F17" s="18"/>
+      <c r="G17" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="24">
+        <v>4</v>
+      </c>
+      <c r="I17" s="20"/>
+    </row>
+    <row r="18" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F18" s="18"/>
+      <c r="G18" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="24">
+        <v>16</v>
+      </c>
+      <c r="I18" s="20"/>
+    </row>
+    <row r="19" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F19" s="18"/>
+      <c r="G19" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="24">
+        <v>4</v>
+      </c>
+      <c r="I19" s="20"/>
+    </row>
+    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F20" s="18"/>
+      <c r="G20" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="24">
+        <v>3</v>
+      </c>
+      <c r="I20" s="20"/>
+    </row>
+    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F21" s="18"/>
+      <c r="G21" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="24">
+        <v>7</v>
+      </c>
+      <c r="I21" s="20"/>
+    </row>
+    <row r="22" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F22" s="18"/>
+      <c r="G22" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="21"/>
+    </row>
+    <row r="23" spans="6:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F23" s="18"/>
+      <c r="G23" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" s="31">
+        <v>4</v>
+      </c>
+      <c r="I23" s="20"/>
+    </row>
+    <row r="24" spans="6:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="18"/>
+      <c r="G24" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H24" s="30">
+        <f>SUM(H17:H23)</f>
+        <v>38</v>
+      </c>
+      <c r="I24" s="18"/>
+    </row>
+    <row r="25" spans="6:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F25" s="18"/>
+      <c r="G25" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="33">
+        <f>H24*0.11</f>
+        <v>4.18</v>
+      </c>
+      <c r="I25" s="18"/>
+    </row>
+    <row r="26" spans="6:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="18"/>
+      <c r="G26" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26" s="27">
+        <v>4</v>
+      </c>
+      <c r="I26" s="18"/>
+    </row>
+    <row r="27" spans="6:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F27" s="18"/>
+      <c r="G27" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27" s="35">
+        <f>H26*0.11</f>
+        <v>0.44</v>
+      </c>
+      <c r="I27" s="18"/>
+    </row>
+    <row r="28" spans="6:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="18"/>
+      <c r="G28" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28" s="36">
+        <v>0.01</v>
+      </c>
+      <c r="I28" s="18"/>
+    </row>
+    <row r="29" spans="6:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F29" s="18"/>
+      <c r="G29" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" s="28">
+        <f>H25+H27+H28</f>
+        <v>4.63</v>
+      </c>
+      <c r="I29" s="18"/>
+    </row>
+    <row r="30" spans="6:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="18"/>
+      <c r="G30" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="H30" s="36">
+        <v>1.64</v>
+      </c>
+      <c r="I30" s="18"/>
+    </row>
+    <row r="31" spans="6:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F31" s="18"/>
+      <c r="G31" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="37">
+        <f>H29+H30</f>
+        <v>6.27</v>
+      </c>
+      <c r="I31" s="18"/>
+    </row>
+    <row r="32" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -777,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,7 +1400,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -958,10 +1407,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>